<commit_message>
debug files for tomorrow
</commit_message>
<xml_diff>
--- a/tracking/ErrorTrackingWorksheetNov15.xlsx
+++ b/tracking/ErrorTrackingWorksheetNov15.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ExecutiveSearchYaml\tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03A3220-3A5F-47F1-85C5-5F5DB96FF7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B409C511-999A-4B50-A821-7895B038221B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18850" yWindow="2410" windowWidth="16710" windowHeight="17860" xr2:uid="{30F64796-086F-4058-892E-0389D3A6EA6C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="190">
   <si>
     <t>FAC</t>
   </si>
@@ -581,10 +581,31 @@
     <t>Seq</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>x</t>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>robotxt</t>
+  </si>
+  <si>
+    <t>templateD</t>
+  </si>
+  <si>
+    <t>Templateed</t>
+  </si>
+  <si>
+    <t>List Item may be solved above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual </t>
+  </si>
+  <si>
+    <t>Blocked</t>
+  </si>
+  <si>
+    <t>?Blocked</t>
+  </si>
+  <si>
+    <t>Review</t>
   </si>
 </sst>
 </file>
@@ -633,7 +654,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -654,15 +675,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FFD6DADC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="medium">
         <color rgb="FFD6DADC"/>
@@ -674,9 +686,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -692,9 +704,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1033,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C2C6452-5DC2-4AB3-84A5-2FAE865E1C3A}">
   <dimension ref="A1:J146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="J96" sqref="J96"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3016,8 +3025,8 @@
       <c r="I62" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J62" s="7" t="s">
-        <v>182</v>
+      <c r="J62" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3049,7 +3058,7 @@
         <v>0</v>
       </c>
       <c r="J63" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3081,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="J64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3113,7 +3122,7 @@
         <v>0</v>
       </c>
       <c r="J65" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3145,7 +3154,7 @@
         <v>0</v>
       </c>
       <c r="J66" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3177,7 +3186,7 @@
         <v>0</v>
       </c>
       <c r="J67" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3209,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="J68" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3241,7 +3250,7 @@
         <v>0</v>
       </c>
       <c r="J69" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3273,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="J70" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3303,7 +3312,7 @@
         <v>4</v>
       </c>
       <c r="J71" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3335,7 +3344,7 @@
         <v>-1</v>
       </c>
       <c r="J72" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3367,7 +3376,7 @@
         <v>0</v>
       </c>
       <c r="J73" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3399,7 +3408,7 @@
         <v>0</v>
       </c>
       <c r="J74" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3431,7 +3440,7 @@
         <v>0</v>
       </c>
       <c r="J75" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3463,7 +3472,7 @@
         <v>0</v>
       </c>
       <c r="J76" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3495,7 +3504,7 @@
         <v>0</v>
       </c>
       <c r="J77" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3527,7 +3536,7 @@
         <v>0</v>
       </c>
       <c r="J78" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3559,7 +3568,7 @@
         <v>0</v>
       </c>
       <c r="J79" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3591,7 +3600,7 @@
         <v>0</v>
       </c>
       <c r="J80" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3623,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="J81" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3655,7 +3664,7 @@
         <v>0</v>
       </c>
       <c r="J82" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3687,7 +3696,7 @@
         <v>0</v>
       </c>
       <c r="J83" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3719,7 +3728,7 @@
         <v>0</v>
       </c>
       <c r="J84" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3751,7 +3760,7 @@
         <v>0</v>
       </c>
       <c r="J85" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3783,7 +3792,7 @@
         <v>0</v>
       </c>
       <c r="J86" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3815,7 +3824,7 @@
         <v>0</v>
       </c>
       <c r="J87" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3847,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="J88" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3879,7 +3888,7 @@
         <v>0</v>
       </c>
       <c r="J89" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3911,7 +3920,7 @@
         <v>0</v>
       </c>
       <c r="J90" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3943,7 +3952,7 @@
         <v>0</v>
       </c>
       <c r="J91" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3975,7 +3984,7 @@
         <v>0</v>
       </c>
       <c r="J92" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4007,7 +4016,7 @@
         <v>1</v>
       </c>
       <c r="J93" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4039,7 +4048,7 @@
         <v>1</v>
       </c>
       <c r="J94" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4071,7 +4080,7 @@
         <v>1</v>
       </c>
       <c r="J95" t="s">
-        <v>10</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4102,8 +4111,11 @@
       <c r="I96" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J96" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -4131,8 +4143,11 @@
       <c r="I97" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J97" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -4160,8 +4175,11 @@
       <c r="I98" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J98" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -4189,8 +4207,11 @@
       <c r="I99" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J99" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -4218,8 +4239,11 @@
       <c r="I100" s="5">
         <v>11</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J100" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -4247,8 +4271,11 @@
       <c r="I101" s="5">
         <v>-2</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J101" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -4276,8 +4303,11 @@
       <c r="I102" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J102" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -4305,8 +4335,11 @@
       <c r="I103" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J103" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -4334,8 +4367,11 @@
       <c r="I104" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J104" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -4363,8 +4399,11 @@
       <c r="I105" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J105" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="4">
         <v>105</v>
       </c>
@@ -4392,8 +4431,11 @@
       <c r="I106" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J106" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="4">
         <v>106</v>
       </c>
@@ -4421,8 +4463,11 @@
       <c r="I107" s="5">
         <v>16</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J107" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -4450,8 +4495,11 @@
       <c r="I108" s="5">
         <v>-1</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J108" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="4">
         <v>108</v>
       </c>
@@ -4479,8 +4527,11 @@
       <c r="I109" s="5">
         <v>-1</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J109" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -4508,8 +4559,11 @@
       <c r="I110" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J110" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -4537,8 +4591,11 @@
       <c r="I111" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J111" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="4">
         <v>111</v>
       </c>
@@ -4566,8 +4623,11 @@
       <c r="I112" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J112" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="4">
         <v>112</v>
       </c>
@@ -4595,8 +4655,11 @@
       <c r="I113" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J113" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="4">
         <v>113</v>
       </c>
@@ -4624,8 +4687,11 @@
       <c r="I114" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J114" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="4">
         <v>114</v>
       </c>
@@ -4653,8 +4719,11 @@
       <c r="I115" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J115" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A116" s="4">
         <v>115</v>
       </c>
@@ -4682,8 +4751,11 @@
       <c r="I116" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J116" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A117" s="4">
         <v>116</v>
       </c>
@@ -4711,8 +4783,11 @@
       <c r="I117" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J117" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A118" s="4">
         <v>117</v>
       </c>
@@ -4740,8 +4815,11 @@
       <c r="I118" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J118" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A119" s="4">
         <v>118</v>
       </c>
@@ -4769,8 +4847,11 @@
       <c r="I119" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J119" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A120" s="4">
         <v>119</v>
       </c>
@@ -4798,8 +4879,11 @@
       <c r="I120" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J120" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A121" s="4">
         <v>120</v>
       </c>
@@ -4827,8 +4911,11 @@
       <c r="I121" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J121" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A122" s="4">
         <v>121</v>
       </c>
@@ -4856,8 +4943,11 @@
       <c r="I122" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J122" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A123" s="4">
         <v>122</v>
       </c>
@@ -4885,8 +4975,11 @@
       <c r="I123" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J123" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A124" s="4">
         <v>123</v>
       </c>
@@ -4914,8 +5007,11 @@
       <c r="I124" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J124" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A125" s="4">
         <v>124</v>
       </c>
@@ -4943,8 +5039,11 @@
       <c r="I125" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J125" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A126" s="4">
         <v>125</v>
       </c>
@@ -4972,8 +5071,11 @@
       <c r="I126" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J126" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A127" s="4">
         <v>126</v>
       </c>
@@ -5001,8 +5103,11 @@
       <c r="I127" s="5">
         <v>-4</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J127" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A128" s="4">
         <v>127</v>
       </c>
@@ -5030,8 +5135,11 @@
       <c r="I128" s="5">
         <v>-1</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J128" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A129" s="4">
         <v>128</v>
       </c>
@@ -5059,8 +5167,11 @@
       <c r="I129" s="5">
         <v>-1</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J129" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A130" s="4">
         <v>129</v>
       </c>
@@ -5088,8 +5199,11 @@
       <c r="I130" s="5">
         <v>-1</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J130" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A131" s="4">
         <v>130</v>
       </c>
@@ -5117,8 +5231,11 @@
       <c r="I131" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J131" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A132" s="4">
         <v>131</v>
       </c>
@@ -5146,8 +5263,11 @@
       <c r="I132" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J132" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A133" s="4">
         <v>132</v>
       </c>
@@ -5175,8 +5295,11 @@
       <c r="I133" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J133" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A134" s="4">
         <v>133</v>
       </c>
@@ -5204,8 +5327,11 @@
       <c r="I134" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J134" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A135" s="4">
         <v>134</v>
       </c>
@@ -5233,8 +5359,11 @@
       <c r="I135" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J135" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A136" s="4">
         <v>135</v>
       </c>
@@ -5262,8 +5391,11 @@
       <c r="I136" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J136" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A137" s="4">
         <v>136</v>
       </c>
@@ -5291,8 +5423,11 @@
       <c r="I137" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J137" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A138" s="4">
         <v>137</v>
       </c>
@@ -5320,8 +5455,11 @@
       <c r="I138" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J138" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A139" s="4">
         <v>138</v>
       </c>
@@ -5349,8 +5487,11 @@
       <c r="I139" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J139" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A140" s="4">
         <v>139</v>
       </c>
@@ -5378,8 +5519,11 @@
       <c r="I140" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J140" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A141" s="4">
         <v>140</v>
       </c>
@@ -5407,8 +5551,11 @@
       <c r="I141" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J141" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A142" s="4">
         <v>141</v>
       </c>
@@ -5436,8 +5583,11 @@
       <c r="I142" s="5">
         <v>-11</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J142" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A143" s="4">
         <v>142</v>
       </c>
@@ -5465,8 +5615,11 @@
       <c r="I143" s="5">
         <v>-8</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J143" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A144" s="4">
         <v>143</v>
       </c>
@@ -5493,6 +5646,9 @@
       </c>
       <c r="I144" s="5">
         <v>-7</v>
+      </c>
+      <c r="J144" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Working through project finalization in preparation for move to post processing branch.I have also moved the old archives file to an ArchiveCode file
</commit_message>
<xml_diff>
--- a/tracking/ErrorTrackingWorksheetNov15.xlsx
+++ b/tracking/ErrorTrackingWorksheetNov15.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ExecutiveSearchYaml\tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B409C511-999A-4B50-A821-7895B038221B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CA9ABD-E8B5-48B0-BF28-DE518F895FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18850" yWindow="2410" windowWidth="16710" windowHeight="17860" xr2:uid="{30F64796-086F-4058-892E-0389D3A6EA6C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="187">
   <si>
     <t>FAC</t>
   </si>
@@ -585,15 +585,6 @@
   </si>
   <si>
     <t>robotxt</t>
-  </si>
-  <si>
-    <t>templateD</t>
-  </si>
-  <si>
-    <t>Templateed</t>
-  </si>
-  <si>
-    <t>List Item may be solved above</t>
   </si>
   <si>
     <t xml:space="preserve">Manual </t>
@@ -1042,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C2C6452-5DC2-4AB3-84A5-2FAE865E1C3A}">
   <dimension ref="A1:J146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J103" sqref="J103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4208,7 +4199,7 @@
         <v>5</v>
       </c>
       <c r="J99" t="s">
-        <v>183</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4304,7 +4295,7 @@
         <v>2</v>
       </c>
       <c r="J102" t="s">
-        <v>184</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4336,7 +4327,7 @@
         <v>4</v>
       </c>
       <c r="J103" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4368,7 +4359,7 @@
         <v>5</v>
       </c>
       <c r="J104" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4400,7 +4391,7 @@
         <v>5</v>
       </c>
       <c r="J105" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4432,7 +4423,7 @@
         <v>6</v>
       </c>
       <c r="J106" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4464,7 +4455,7 @@
         <v>16</v>
       </c>
       <c r="J107" t="s">
-        <v>185</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4496,7 +4487,7 @@
         <v>-1</v>
       </c>
       <c r="J108" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4528,7 +4519,7 @@
         <v>-1</v>
       </c>
       <c r="J109" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4560,7 +4551,7 @@
         <v>0</v>
       </c>
       <c r="J110" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="111" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4592,7 +4583,7 @@
         <v>0</v>
       </c>
       <c r="J111" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="112" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4624,7 +4615,7 @@
         <v>0</v>
       </c>
       <c r="J112" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4656,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="J113" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="114" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4688,7 +4679,7 @@
         <v>0</v>
       </c>
       <c r="J114" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4720,7 +4711,7 @@
         <v>0</v>
       </c>
       <c r="J115" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4752,7 +4743,7 @@
         <v>0</v>
       </c>
       <c r="J116" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4784,7 +4775,7 @@
         <v>0</v>
       </c>
       <c r="J117" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4816,7 +4807,7 @@
         <v>0</v>
       </c>
       <c r="J118" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4848,7 +4839,7 @@
         <v>0</v>
       </c>
       <c r="J119" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4880,7 +4871,7 @@
         <v>0</v>
       </c>
       <c r="J120" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="121" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4912,7 +4903,7 @@
         <v>4</v>
       </c>
       <c r="J121" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4944,7 +4935,7 @@
         <v>4</v>
       </c>
       <c r="J122" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="123" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -5651,7 +5642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A145" s="4">
         <v>144</v>
       </c>
@@ -5679,8 +5670,11 @@
       <c r="I145" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" ht="32" x14ac:dyDescent="0.35">
+      <c r="J145" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" ht="32" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>178</v>
       </c>

</xml_diff>